<commit_message>
Resolution of father/mother cross-references
</commit_message>
<xml_diff>
--- a/model/family.xlsx
+++ b/model/family.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Feature</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Date of birth</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Mother</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -495,7 +501,7 @@
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -508,8 +514,14 @@
       <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -520,7 +532,7 @@
         <v>17236</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -528,7 +540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -536,23 +548,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -560,44 +584,62 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>